<commit_message>
Added jsonReader to code Added assertion is added
</commit_message>
<xml_diff>
--- a/Framework/src/main/resources/Book1.xlsx
+++ b/Framework/src/main/resources/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\TestingFramework\Framework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8F8681-C484-4D89-97EA-7AB25B5DF2D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD5442-4418-43A3-9672-84BDE1005234}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="-108" windowWidth="29016" windowHeight="15816" xr2:uid="{493A33BC-4A3B-497A-AA7F-DDF0CBBAE924}"/>
+    <workbookView xWindow="3864" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{493A33BC-4A3B-497A-AA7F-DDF0CBBAE924}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,80 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Mones</t>
+    <t>Execute</t>
   </si>
   <si>
-    <t>sddsdudifu</t>
+    <t>https://www.google.com/</t>
   </si>
   <si>
-    <t>erfref</t>
+    <t>Address</t>
   </si>
   <si>
-    <t>erf</t>
+    <t>https://dog.ceo/api/breeds/image/random</t>
   </si>
   <si>
-    <t>fer</t>
-  </si>
-  <si>
-    <t>fref</t>
-  </si>
-  <si>
-    <t>ferf</t>
-  </si>
-  <si>
-    <t>fre</t>
-  </si>
-  <si>
-    <t>fdsf</t>
-  </si>
-  <si>
-    <t>reg</t>
-  </si>
-  <si>
-    <t>dwe</t>
-  </si>
-  <si>
-    <t>ewd</t>
-  </si>
-  <si>
-    <t>dew</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>wed</t>
-  </si>
-  <si>
-    <t>wde</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>dwwe</t>
-  </si>
-  <si>
-    <t>edw</t>
-  </si>
-  <si>
-    <t>ew</t>
-  </si>
-  <si>
-    <t>dewd</t>
-  </si>
-  <si>
-    <t>ed</t>
+    <t>https://dog.ceo/api/breeds/list/all</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,8 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,175 +403,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D31A5F-9CF5-4957-857C-24190F382A2E}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.88671875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B4" t="b">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>4252</v>
-      </c>
-      <c r="I2">
-        <v>25424554</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>12242</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3">
-        <v>121</v>
-      </c>
-      <c r="K3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4">
-        <v>1212</v>
-      </c>
-      <c r="K4">
-        <v>121</v>
-      </c>
-      <c r="L4">
-        <v>1213</v>
-      </c>
-      <c r="M4">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L5">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated switch case for move element and select
</commit_message>
<xml_diff>
--- a/Framework/src/main/resources/Book1.xlsx
+++ b/Framework/src/main/resources/Book1.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\TestingFramework\Framework\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TestingFramework\Framework\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD5442-4418-43A3-9672-84BDE1005234}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E136EBE0-676D-4F6F-8DE3-36AAFABFAE0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3864" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{493A33BC-4A3B-497A-AA7F-DDF0CBBAE924}"/>
+    <workbookView xWindow="2265" yWindow="570" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{493A33BC-4A3B-497A-AA7F-DDF0CBBAE924}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="API" sheetId="1" r:id="rId1"/>
+    <sheet name="WebElement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Execute</t>
   </si>
@@ -40,13 +41,37 @@
   </si>
   <si>
     <t>https://dog.ceo/api/breeds/list/all</t>
+  </si>
+  <si>
+    <t>Attributes</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>googleTextfield</t>
+  </si>
+  <si>
+    <t>googlebuttonSearch</t>
+  </si>
+  <si>
+    <t>btnK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +86,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,12 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,17 +438,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1D31A5F-9CF5-4957-857C-24190F382A2E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -423,7 +456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -431,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -439,7 +472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -451,4 +484,58 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD0E5D1-D529-43EA-AA48-7D0873706251}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>